<commit_message>
fixed json fields for conversion to slx
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32" count="32">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17" count="17">
   <x:si>
     <x:t>message</x:t>
   </x:si>
@@ -22,94 +22,49 @@
     <x:t>site</x:t>
   </x:si>
   <x:si>
-    <x:t>ip_addr</x:t>
-  </x:si>
-  <x:si>
-    <x:t>in_cf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>name_servers</x:t>
-  </x:si>
-  <x:si>
-    <x:t>original_name_servers</x:t>
-  </x:si>
-  <x:si>
-    <x:t>original_registrar</x:t>
-  </x:si>
-  <x:si>
-    <x:t>mx records</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CF &amp; DNS check initiated at Mon Aug 16 2021 15:30:21 GMT-0600 (Mountain Daylight Time)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>n/a</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CF / DNS check completed at Mon Aug 16 2021 15:30:23 GMT-0600 (Mountain Daylight Time)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2 of 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>aeacleaningservices.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>163.182.168.98</x:t>
-  </x:si>
-  <x:si>
-    <x:t>no</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Pointed IP: 163.182.168.98</x:t>
-  </x:si>
-  <x:si>
-    <x:t>data not available</x:t>
-  </x:si>
-  <x:si>
-    <x:t>no mx records found</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3 of 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>akrosteam.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>163.182.168.98</x:t>
-  </x:si>
-  <x:si>
-    <x:t>yes</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ivan.ns.cloudflare.com,lina.ns.cloudflare.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ns11.domaincontrol.com,ns12.domaincontrol.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>godaddy.com, llc (id: 146)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>exchange: ALT1.ASPMX.L.GOOGLE.com, priority: 5,exchange: ALT2.ASPMX.L.GOOGLE.com, priority: 5,exchange: ASPMX.L.GOOGLE.com, priority: 1,exchange: ASPMX2.GOOGLEMAIL.com, priority: 10,exchange: ASPMX3.GOOGLEMAIL.com, priority: 10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1 of 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>advancedcarpetcleaningandrestoration.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>172.67.174.24,104.21.64.13</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ivan.ns.cloudflare.com,lina.ns.cloudflare.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ns1.bigwesthost.com,ns2.bigwesthost.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>no mx records found</x:t>
+    <x:t>data_type</x:t>
+  </x:si>
+  <x:si>
+    <x:t>datum</x:t>
+  </x:si>
+  <x:si>
+    <x:t>H scrape initiated at Wed Aug 18 2021 13:24:15 GMT-0600 (Mountain Daylight Time)</x:t>
+  </x:si>
+  <x:si>
+    <x:t/>
+  </x:si>
+  <x:si>
+    <x:t>https://bigwestplayground.com/theultimatic</x:t>
+  </x:si>
+  <x:si>
+    <x:t>h1</x:t>
+  </x:si>
+  <x:si>
+    <x:t> Home</x:t>
+  </x:si>
+  <x:si>
+    <x:t> Javascriptless Before/After Slider</x:t>
+  </x:si>
+  <x:si>
+    <x:t> Category + Keywords</x:t>
+  </x:si>
+  <x:si>
+    <x:t>h2</x:t>
+  </x:si>
+  <x:si>
+    <x:t> Welcome to BIZ NAME</x:t>
+  </x:si>
+  <x:si>
+    <x:t> Sub-Heading</x:t>
+  </x:si>
+  <x:si>
+    <x:t> Reviews from Our Clients</x:t>
+  </x:si>
+  <x:si>
+    <x:t> Connect with Us</x:t>
+  </x:si>
+  <x:si>
+    <x:t>H scrape completed at Wed Aug 18 2021 13:24:17 GMT-0600 (Mountain Daylight Time)</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -472,7 +427,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:8">
+    <x:row r="1" spans="1:4">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -485,144 +440,131 @@
       <x:c r="D1" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E1" s="0" t="s">
+    </x:row>
+    <x:row r="2" spans="1:4">
+      <x:c r="A2" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="F1" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="G1" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="H1" s="0" t="s">
+      <x:c r="B2" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:4">
+      <x:c r="A3" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:8">
-      <x:c r="A2" s="0" t="s">
+      <x:c r="D3" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="B2" s="0" t="s">
+    </x:row>
+    <x:row r="4" spans="1:4">
+      <x:c r="A4" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="E2" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="F2" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="G2" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="H2" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:8">
-      <x:c r="A3" s="0" t="s">
+    </x:row>
+    <x:row r="5" spans="1:4">
+      <x:c r="A5" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="F3" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="G3" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="H3" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:8">
-      <x:c r="A4" s="0" t="s">
+    </x:row>
+    <x:row r="6" spans="1:4">
+      <x:c r="A6" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="B4" s="0" t="s">
+      <x:c r="D6" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="C4" s="0" t="s">
+    </x:row>
+    <x:row r="7" spans="1:4">
+      <x:c r="A7" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="D4" s="0" t="s">
+    </x:row>
+    <x:row r="8" spans="1:4">
+      <x:c r="A8" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="E4" s="0" t="s">
+    </x:row>
+    <x:row r="9" spans="1:4">
+      <x:c r="A9" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="F4" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="G4" s="0" t="s">
+    </x:row>
+    <x:row r="10" spans="1:4">
+      <x:c r="A10" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="H4" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:8">
-      <x:c r="A5" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="D5" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="E5" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="F5" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="G5" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="H5" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:8">
-      <x:c r="A6" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="D6" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="E6" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="F6" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="H6" s="0" t="s">
-        <x:v>31</x:v>
+      <x:c r="B10" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>5</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>